<commit_message>
Create rules and plot
Created rules for each category and products (both retailers and corporates). And also tried to plot the new rules generated.
</commit_message>
<xml_diff>
--- a/Datasets/ElectronidexItems2017.xlsx
+++ b/Datasets/ElectronidexItems2017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelriberazaragoza/Documents/Ubiqum/WEEK 7/Market-Basket-Analysis/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA78A698-A3F2-F34B-9DDB-B530C62EDC60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78231580-4733-F541-8552-D428D90F5DD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -978,7 +978,7 @@
   <dimension ref="A1:D146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1004,346 +1004,349 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>154</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C2" s="4"/>
       <c r="D2">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>142</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>175</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>79</v>
+      <c r="A6" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C6" s="4"/>
       <c r="D6">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>750</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="D10">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>80</v>
+      <c r="A11" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="D12">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>84</v>
+      <c r="A13" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D14">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D15">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D16">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>148</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D19">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D20">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D21">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="D22">
-        <v>50</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="D23">
-        <v>50</v>
+        <v>750</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="D24">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>175</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="D27">
         <v>50</v>
@@ -1351,41 +1354,41 @@
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D28">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="D29">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="D30">
         <v>50</v>
@@ -1393,698 +1396,711 @@
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="D31">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="D32">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="D33">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>166</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C35" s="4"/>
       <c r="D35">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D36">
-        <v>50</v>
+        <v>750</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D37">
-        <v>50</v>
+        <v>750</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="D38">
-        <v>50</v>
+        <v>750</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="D39">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="D40">
-        <v>50</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="D41">
-        <v>25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>118</v>
+        <v>43</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D42">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D43">
-        <v>25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="D44">
-        <v>25</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="D45">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>124</v>
+        <v>53</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D46">
-        <v>300</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D47">
-        <v>300</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D48">
-        <v>300</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="D49">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="D50">
-        <v>300</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>143</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C51" s="4"/>
       <c r="D51">
-        <v>750</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="D52">
-        <v>750</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D53">
-        <v>750</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>155</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C54" s="4"/>
       <c r="D54">
-        <v>750</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>155</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C55" s="4"/>
       <c r="D55">
-        <v>750</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>166</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C56" s="4"/>
       <c r="D56">
-        <v>750</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="D57">
-        <v>750</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D58">
-        <v>750</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D59">
-        <v>750</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C62" s="4"/>
+        <v>118</v>
+      </c>
       <c r="D62">
-        <v>75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C63" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="D63">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="D64">
-        <v>75</v>
+        <v>750</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="D65">
-        <v>35</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="D66">
-        <v>35</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="D67">
-        <v>35</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C68" s="4"/>
+      <c r="C68" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="D68">
         <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D69">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>166</v>
       </c>
       <c r="D70">
-        <v>35</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="D71">
-        <v>35</v>
+        <v>750</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D72">
-        <v>35</v>
+        <v>750</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="D73">
-        <v>35</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D74">
-        <v>1000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D75">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="D76">
-        <v>1000</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="D77">
-        <v>1000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="D78">
-        <v>1000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D79">
-        <v>1000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="D80">
-        <v>1000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D81">
-        <v>1000</v>
+        <v>750</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D82">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2103,220 +2119,223 @@
     </row>
     <row r="84" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="D84">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="D85">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="D86">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="D87">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="D88">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="D89">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D90">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D91">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D92">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="D93">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="D94">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D95">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D96">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D97">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D98">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D99">
         <v>60</v>
@@ -2324,7 +2343,7 @@
     </row>
     <row r="100" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>53</v>
@@ -2338,41 +2357,35 @@
     </row>
     <row r="101" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="D101">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>179</v>
+        <v>118</v>
       </c>
       <c r="D102">
-        <v>60</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>151</v>
+        <v>74</v>
       </c>
       <c r="D103">
         <v>50</v>
@@ -2380,13 +2393,13 @@
     </row>
     <row r="104" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="D104">
         <v>50</v>
@@ -2394,13 +2407,13 @@
     </row>
     <row r="105" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="D105">
         <v>50</v>
@@ -2408,27 +2421,27 @@
     </row>
     <row r="106" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D106">
         <v>50</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
-        <v>114</v>
+      <c r="A107" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="D107">
         <v>50</v>
@@ -2436,161 +2449,156 @@
     </row>
     <row r="108" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="D108">
-        <v>250</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="D109">
-        <v>250</v>
+        <v>60</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="D110">
-        <v>250</v>
+        <v>35</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D111">
-        <v>250</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="D112">
-        <v>250</v>
+        <v>80</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>136</v>
+        <v>81</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="D113">
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="D114">
-        <v>80</v>
+        <v>300</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>138</v>
+        <v>27</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>136</v>
+        <v>21</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="D115">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>141</v>
+        <v>28</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>136</v>
+        <v>21</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D116">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>136</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C117" s="4"/>
       <c r="D117">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>150</v>
+        <v>32</v>
       </c>
       <c r="D118">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="D119">
         <v>80</v>
@@ -2598,98 +2606,90 @@
     </row>
     <row r="120" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C120" s="4"/>
+      <c r="C120" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D120">
         <v>80</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>156</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C121" s="4"/>
       <c r="D121">
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>168</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C122" s="4"/>
       <c r="D122">
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D123">
         <v>100</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D123">
-        <v>80</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>174</v>
+        <v>32</v>
       </c>
       <c r="D124">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D125">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>105</v>
+        <v>184</v>
       </c>
       <c r="D126">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2713,8 +2713,8 @@
     <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D148">
-    <sortCondition ref="B1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D146">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>